<commit_message>
screenshots added, file tree cleanup
</commit_message>
<xml_diff>
--- a/log_book2.xlsx
+++ b/log_book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7494085B-729C-40CB-94A9-25A5D07F2956}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECD6E0E-2D6A-4B7A-9A2F-E6DB6E90A1DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,23 @@
     <sheet name="Facts" sheetId="2" r:id="rId2"/>
     <sheet name="Projects" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="189">
   <si>
     <t>Description</t>
   </si>
@@ -588,6 +594,12 @@
   </si>
   <si>
     <t>Clean up the files, prepare /dist folder for final program. Push latest version to GITHUB</t>
+  </si>
+  <si>
+    <t>Total tasks:</t>
+  </si>
+  <si>
+    <t>Tasks left:</t>
   </si>
 </sst>
 </file>
@@ -597,7 +609,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,8 +682,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,8 +712,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -821,15 +845,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -950,13 +990,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="5" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Blogas" xfId="2" builtinId="27"/>
     <cellStyle name="Geras" xfId="1" builtinId="26"/>
     <cellStyle name="Hipersaitas" xfId="3" builtinId="8"/>
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
     <cellStyle name="Neutralus" xfId="4" builtinId="28"/>
+    <cellStyle name="Pastaba" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1303,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
-  <dimension ref="B1:H48"/>
+  <dimension ref="B1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1320,72 +1367,65 @@
     <col min="8" max="8" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="54">
+        <f>COUNTIF(B4:B149, "&lt;&gt;")</f>
+        <v>45</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="55">
+        <f>C1 - COUNTIF(D4:D74,  "&lt;&gt;")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -1399,172 +1439,172 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>54</v>
+      <c r="D7" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="C9" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="D9" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>56</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>118</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D10" s="45"/>
       <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C13" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
         <v>68</v>
       </c>
@@ -1574,91 +1614,94 @@
       <c r="D14" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>69</v>
+      <c r="E14" t="s">
+        <v>67</v>
       </c>
       <c r="F14" t="s">
         <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="24" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>101</v>
+      <c r="D15" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C17" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D17" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+    <row r="18" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C18" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D18" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E18" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1668,214 +1711,211 @@
       <c r="C19" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>79</v>
+      <c r="D19" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
         <v>92</v>
       </c>
       <c r="C21" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D22" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>91</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>166</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="24" t="s">
         <v>95</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D23" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B24" s="24" t="s">
         <v>95</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" t="s">
-        <v>170</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>171</v>
+      <c r="E24" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C26" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D26" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>154</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H26" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="46" t="s">
+    <row r="27" spans="2:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C27" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D27" s="47">
         <v>44137</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E27" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F27" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G27" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="48" t="s">
+      <c r="H27" s="48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="41" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C28" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D28" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E28" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="43" t="s">
+      <c r="F28" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-    </row>
-    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" t="s">
-        <v>137</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" t="s">
-        <v>151</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+    </row>
+    <row r="29" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>137</v>
       </c>
@@ -1886,10 +1926,16 @@
         <v>137</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F29" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="G29" t="s">
+        <v>151</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -1903,35 +1949,33 @@
         <v>137</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>150</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="38" t="s">
         <v>95</v>
       </c>
@@ -1942,214 +1986,221 @@
         <v>140</v>
       </c>
       <c r="E32" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F33" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G33" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="H32" s="27"/>
-    </row>
-    <row r="33" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B33" s="34" t="s">
+      <c r="H33" s="27"/>
+    </row>
+    <row r="34" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B34" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C34" s="40">
         <v>44167</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D34" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C34" s="40"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="1" t="s">
+    <row r="35" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C35" s="40"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B35" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F35" t="s">
-        <v>178</v>
-      </c>
-      <c r="G35" t="s">
-        <v>176</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B36" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="44"/>
+      <c r="E36" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D37" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>157</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="49" t="s">
+    <row r="38" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C38" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D38" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E38" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="51" t="s">
+      <c r="F38" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="G37" s="51" t="s">
+      <c r="G38" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="H37" s="50"/>
-    </row>
-    <row r="38" spans="2:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B38" s="34" t="s">
+      <c r="H38" s="50"/>
+    </row>
+    <row r="39" spans="2:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D39" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E39" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="34" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C40" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D40" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="37" t="s">
+      <c r="E40" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>138</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>139</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D40" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="E40" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="F40" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="40">
-        <v>43985</v>
-      </c>
-      <c r="D41" s="44"/>
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>163</v>
+      </c>
       <c r="E41" s="37" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B42" s="40">
-        <v>43985</v>
+        <v>160</v>
+      </c>
+      <c r="F41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="C42" s="40">
         <v>43985</v>
       </c>
-      <c r="D42" s="53">
-        <v>43985</v>
-      </c>
-      <c r="E42" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D42" s="44"/>
+      <c r="E42" s="37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B43" s="40">
         <v>43985</v>
       </c>
       <c r="C43" s="40">
         <v>43985</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="37" t="s">
-        <v>181</v>
+      <c r="D43" s="53">
+        <v>43985</v>
+      </c>
+      <c r="E43" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
@@ -2160,8 +2211,8 @@
         <v>43985</v>
       </c>
       <c r="D44" s="44"/>
-      <c r="E44" s="1" t="s">
-        <v>182</v>
+      <c r="E44" s="37" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
@@ -2173,16 +2224,19 @@
       </c>
       <c r="D45" s="44"/>
       <c r="E45" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="40">
         <v>43985</v>
       </c>
+      <c r="C46" s="40">
+        <v>43985</v>
+      </c>
       <c r="D46" s="44"/>
       <c r="E46" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
@@ -2191,18 +2245,27 @@
       </c>
       <c r="D47" s="44"/>
       <c r="E47" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="40">
         <v>43985</v>
       </c>
-      <c r="C48" s="40">
-        <v>43985</v>
-      </c>
       <c r="D48" s="44"/>
       <c r="E48" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="40">
+        <v>43985</v>
+      </c>
+      <c r="C49" s="40">
+        <v>43985</v>
+      </c>
+      <c r="D49" s="44"/>
+      <c r="E49" s="1" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ability to change color schema specifications deep update v1.4 logbook update
</commit_message>
<xml_diff>
--- a/log_book2.xlsx
+++ b/log_book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECD6E0E-2D6A-4B7A-9A2F-E6DB6E90A1DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C72A051-B057-4CD2-823B-1DA844539934}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="195">
   <si>
     <t>Description</t>
   </si>
@@ -600,6 +600,24 @@
   </si>
   <si>
     <t>Tasks left:</t>
+  </si>
+  <si>
+    <t>Final data flowdiagram created</t>
+  </si>
+  <si>
+    <t>Update the specifications</t>
+  </si>
+  <si>
+    <t>Had to rework the DFD from the ground</t>
+  </si>
+  <si>
+    <t>14/3/2020</t>
+  </si>
+  <si>
+    <t>Production ready code Pushed to github</t>
+  </si>
+  <si>
+    <t>Write report about it</t>
   </si>
 </sst>
 </file>
@@ -1352,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
   <dimension ref="B1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,7 +1398,7 @@
       </c>
       <c r="E1" s="55">
         <f>C1 - COUNTIF(D4:D74,  "&lt;&gt;")</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2053,7 +2071,12 @@
       <c r="B36" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="44"/>
+      <c r="C36" s="40">
+        <v>43832</v>
+      </c>
+      <c r="D36" s="53">
+        <v>44167</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>173</v>
       </c>
@@ -2210,9 +2233,20 @@
       <c r="C44" s="40">
         <v>43985</v>
       </c>
-      <c r="D44" s="44"/>
+      <c r="D44" s="53">
+        <v>44107</v>
+      </c>
       <c r="E44" s="37" t="s">
         <v>181</v>
+      </c>
+      <c r="F44" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H44" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
@@ -2257,16 +2291,24 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" s="40">
         <v>43985</v>
       </c>
       <c r="C49" s="40">
         <v>43985</v>
       </c>
-      <c r="D49" s="44"/>
+      <c r="D49" s="36" t="s">
+        <v>192</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>186</v>
+      </c>
+      <c r="F49" t="s">
+        <v>193</v>
+      </c>
+      <c r="G49" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new specifications doc release
</commit_message>
<xml_diff>
--- a/log_book2.xlsx
+++ b/log_book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C72A051-B057-4CD2-823B-1DA844539934}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0238C0A-0EE3-4E10-BAB4-A32DF8707459}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="207">
   <si>
     <t>Description</t>
   </si>
@@ -618,6 +618,42 @@
   </si>
   <si>
     <t>Write report about it</t>
+  </si>
+  <si>
+    <t>16/03/2020</t>
+  </si>
+  <si>
+    <t>INSTALL.md file explains how to run this software</t>
+  </si>
+  <si>
+    <t>Start writing final report</t>
+  </si>
+  <si>
+    <t>Didn’t know how much in detail I need to explain. Depends on the audience. Assumed that reader is semi skilled</t>
+  </si>
+  <si>
+    <t>Color support/ including color schema for blind people</t>
+  </si>
+  <si>
+    <t>20/03/2020</t>
+  </si>
+  <si>
+    <t>Code is working and pushed on github</t>
+  </si>
+  <si>
+    <t>Mention about it in the report</t>
+  </si>
+  <si>
+    <t>Completely rewrote the specifications, eliminated I, we etc. SMART target list is still missing</t>
+  </si>
+  <si>
+    <t>Complete the SMART list</t>
+  </si>
+  <si>
+    <t>Don’t know how to write SMART list, need lecturer assistance</t>
+  </si>
+  <si>
+    <t>Have a paper note with the topics to write about. Also read the marking criteria</t>
   </si>
 </sst>
 </file>
@@ -1368,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
-  <dimension ref="B1:H49"/>
+  <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,14 +1427,14 @@
       </c>
       <c r="C1" s="54">
         <f>COUNTIF(B4:B149, "&lt;&gt;")</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>188</v>
       </c>
       <c r="E1" s="55">
         <f>C1 - COUNTIF(D4:D74,  "&lt;&gt;")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2194,16 +2230,27 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B42" s="34" t="s">
         <v>137</v>
       </c>
       <c r="C42" s="40">
         <v>43985</v>
       </c>
-      <c r="D42" s="44"/>
+      <c r="D42" s="36" t="s">
+        <v>195</v>
+      </c>
       <c r="E42" s="37" t="s">
         <v>161</v>
+      </c>
+      <c r="F42" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" t="s">
+        <v>197</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2249,28 +2296,44 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="40">
         <v>43985</v>
       </c>
       <c r="C45" s="40">
         <v>43985</v>
       </c>
-      <c r="D45" s="44"/>
+      <c r="D45" s="36" t="s">
+        <v>200</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F45" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45" t="s">
+        <v>204</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B46" s="40">
         <v>43985</v>
       </c>
       <c r="C46" s="40">
         <v>43985</v>
       </c>
-      <c r="D46" s="44"/>
+      <c r="D46" s="25" t="s">
+        <v>200</v>
+      </c>
       <c r="E46" s="1" t="s">
         <v>185</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
@@ -2309,6 +2372,26 @@
       </c>
       <c r="G49" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F50" t="s">
+        <v>201</v>
+      </c>
+      <c r="G50" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
specifications update, images folder added
</commit_message>
<xml_diff>
--- a/log_book2.xlsx
+++ b/log_book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0238C0A-0EE3-4E10-BAB4-A32DF8707459}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5DC68B-5BD1-4C25-9E5C-1E9F6EFE434F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work plan" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="208">
   <si>
     <t>Description</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>Have a paper note with the topics to write about. Also read the marking criteria</t>
+  </si>
+  <si>
+    <t>22/03/2020</t>
   </si>
 </sst>
 </file>
@@ -923,7 +926,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1023,9 +1026,6 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,19 +1422,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="55" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="54">
+      <c r="C1" s="53">
         <f>COUNTIF(B4:B149, "&lt;&gt;")</f>
         <v>46</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="55">
+      <c r="E1" s="54">
         <f>C1 - COUNTIF(D4:D74,  "&lt;&gt;")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1595,7 +1595,9 @@
       <c r="C10" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="28" t="s">
+        <v>207</v>
+      </c>
       <c r="E10" t="s">
         <v>58</v>
       </c>
@@ -1928,25 +1930,25 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <v>44137</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="H27" s="47" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2110,7 +2112,7 @@
       <c r="C36" s="40">
         <v>43832</v>
       </c>
-      <c r="D36" s="53">
+      <c r="D36" s="52">
         <v>44167</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -2147,25 +2149,25 @@
       </c>
     </row>
     <row r="38" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="51" t="s">
+      <c r="F38" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="G38" s="51" t="s">
+      <c r="G38" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="H38" s="50"/>
+      <c r="H38" s="49"/>
     </row>
     <row r="39" spans="2:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B39" s="34" t="s">
@@ -2260,10 +2262,10 @@
       <c r="C43" s="40">
         <v>43985</v>
       </c>
-      <c r="D43" s="53">
+      <c r="D43" s="52">
         <v>43985</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="51" t="s">
         <v>132</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -2280,7 +2282,7 @@
       <c r="C44" s="40">
         <v>43985</v>
       </c>
-      <c r="D44" s="53">
+      <c r="D44" s="52">
         <v>44107</v>
       </c>
       <c r="E44" s="37" t="s">
@@ -2404,7 +2406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA740113-872B-4F20-AC91-9037BB06D52F}">
   <dimension ref="A3:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>